<commit_message>
Fix error in GetDetails.java
</commit_message>
<xml_diff>
--- a/SearchOption1/Email_List_Indexes.xlsx
+++ b/SearchOption1/Email_List_Indexes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationSearchJoB\SearchOption1\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -40,6 +40,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,9 +405,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.77734375"/>
+    <col min="2" max="2" customWidth="true" width="19.88671875"/>
+    <col min="3" max="3" customWidth="true" width="20.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.35">
@@ -421,14 +422,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="24.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2</v>
+      <c r="A2" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Change all the file from the GUI that give me trnasfer the data from the user to web
</commit_message>
<xml_diff>
--- a/SearchOption1/Email_List_Indexes.xlsx
+++ b/SearchOption1/Email_List_Indexes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationSearchJoB\SearchOption1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C3A0A4-3A6B-464C-B818-BA6254AE1873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F63F79-211C-46BD-8036-134A23AD1695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -40,7 +40,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -400,14 +399,14 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.77734375"/>
-    <col min="2" max="2" customWidth="true" width="19.88671875"/>
-    <col min="3" max="3" customWidth="true" width="20.0"/>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.35">
@@ -422,14 +421,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="24.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>2.0</v>
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>